<commit_message>
Version 1. Pretested and cleaned
</commit_message>
<xml_diff>
--- a/cases/fakecaselinelist_2021-07-16.xlsx
+++ b/cases/fakecaselinelist_2021-07-16.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,15 +428,15 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>44980</v>
+        <v>12579</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Amal Ford</t>
+          <t>Elijah Henson</t>
         </is>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -445,33 +445,39 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Grand Wellworth</t>
+          <t>Mexe</t>
         </is>
       </c>
       <c r="F2" s="2">
-        <v>44392</v>
+        <v>44380</v>
       </c>
       <c r="G2" s="2">
-        <v>44392</v>
+        <v>44381</v>
+      </c>
+      <c r="H2" s="2">
+        <v>44387</v>
+      </c>
+      <c r="I2" s="2">
+        <v>44388</v>
       </c>
       <c r="J2" s="2">
-        <v>44387</v>
+        <v>44379</v>
       </c>
       <c r="K2" s="2">
-        <v>44392.66666666667</v>
+        <v>44382</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>44997</v>
+        <v>13289</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Penelope Fields</t>
+          <t>Ella-Mai Gregory</t>
         </is>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -480,69 +486,78 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mexe</t>
+          <t>Grand Wellworth</t>
         </is>
       </c>
       <c r="F3" s="2">
-        <v>44392</v>
+        <v>44379</v>
       </c>
       <c r="G3" s="2">
-        <v>44393</v>
+        <v>44380</v>
+      </c>
+      <c r="J3" s="2">
+        <v>44379</v>
       </c>
       <c r="K3" s="2">
-        <v>44392.66666666667</v>
+        <v>44381</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>44986</v>
+        <v>13479</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Martin F Romero</t>
+          <t>Ceara West</t>
         </is>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Port Sipleach</t>
+          <t>Chorgains</t>
         </is>
       </c>
       <c r="F4" s="2">
-        <v>44392</v>
+        <v>44378</v>
       </c>
       <c r="G4" s="2">
-        <v>44392</v>
+        <v>44379</v>
+      </c>
+      <c r="H4" s="2">
+        <v>44392</v>
+      </c>
+      <c r="I4" s="2">
+        <v>44393</v>
       </c>
       <c r="J4" s="2">
-        <v>44389</v>
+        <v>44378</v>
       </c>
       <c r="K4" s="2">
-        <v>44392.66666666667</v>
+        <v>44380</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>44992</v>
+        <v>13547</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jessica Bauer</t>
+          <t>Francissek Vickers</t>
         </is>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -551,50 +566,374 @@
         </is>
       </c>
       <c r="F5" s="2">
-        <v>44392</v>
+        <v>44387</v>
       </c>
       <c r="G5" s="2">
-        <v>44392</v>
+        <v>44388</v>
+      </c>
+      <c r="H5" s="2">
+        <v>44392</v>
+      </c>
+      <c r="I5" s="2">
+        <v>44393</v>
       </c>
       <c r="J5" s="2">
         <v>44387</v>
       </c>
       <c r="K5" s="2">
-        <v>44392.66666666667</v>
+        <v>44389</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
+        <v>13566</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Penelope F. Fields</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>San Wadhor</t>
+        </is>
+      </c>
+      <c r="F6" s="2">
+        <v>44379</v>
+      </c>
+      <c r="G6" s="2">
+        <v>44379</v>
+      </c>
+      <c r="J6" s="2">
+        <v>44378</v>
+      </c>
+      <c r="K6" s="2">
+        <v>44380</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>13597</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Agata Lucas</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>35</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Port Sipleach</t>
+        </is>
+      </c>
+      <c r="F7" s="2">
+        <v>44379</v>
+      </c>
+      <c r="G7" s="2">
+        <v>44380</v>
+      </c>
+      <c r="J7" s="2">
+        <v>44377</v>
+      </c>
+      <c r="K7" s="2">
+        <v>44381</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>13788</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Eve M. Mcbride</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>58</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>San Wadhor</t>
+        </is>
+      </c>
+      <c r="F8" s="2">
+        <v>44379</v>
+      </c>
+      <c r="G8" s="2">
+        <v>44379</v>
+      </c>
+      <c r="J8" s="2">
+        <v>44377</v>
+      </c>
+      <c r="K8" s="2">
+        <v>44380</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>18400</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Leonidas Hudson</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Eastmsallbuck Creek</t>
+        </is>
+      </c>
+      <c r="F9" s="2">
+        <v>44384</v>
+      </c>
+      <c r="G9" s="2">
+        <v>44385</v>
+      </c>
+      <c r="H9" s="2">
+        <v>44392</v>
+      </c>
+      <c r="I9" s="2">
+        <v>44392</v>
+      </c>
+      <c r="J9" s="2">
+        <v>44383</v>
+      </c>
+      <c r="K9" s="2">
+        <v>44386</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>18793</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Dustin Payne</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Grand Wellworth</t>
+        </is>
+      </c>
+      <c r="F10" s="2">
+        <v>44385</v>
+      </c>
+      <c r="G10" s="2">
+        <v>44386</v>
+      </c>
+      <c r="J10" s="2">
+        <v>44385</v>
+      </c>
+      <c r="K10" s="2">
+        <v>44387</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>44980</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Amal Ford</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Grand Wellworth</t>
+        </is>
+      </c>
+      <c r="F11" s="2">
+        <v>44392</v>
+      </c>
+      <c r="G11" s="2">
+        <v>44392</v>
+      </c>
+      <c r="J11" s="2">
+        <v>44387</v>
+      </c>
+      <c r="K11" s="2">
+        <v>44392.66666666667</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>44986</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Martin F Romero</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Port Sipleach</t>
+        </is>
+      </c>
+      <c r="F12" s="2">
+        <v>44392</v>
+      </c>
+      <c r="G12" s="2">
+        <v>44392</v>
+      </c>
+      <c r="J12" s="2">
+        <v>44389</v>
+      </c>
+      <c r="K12" s="2">
+        <v>44392.66666666667</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
         <v>44990</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Fern Christian Mcarthur</t>
         </is>
       </c>
-      <c r="C6">
+      <c r="C13">
         <v>40</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Port Sipleach</t>
         </is>
       </c>
-      <c r="F6" s="2">
-        <v>44392</v>
-      </c>
-      <c r="G6" s="2">
-        <v>44392</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="F13" s="2">
+        <v>44392</v>
+      </c>
+      <c r="G13" s="2">
+        <v>44392</v>
+      </c>
+      <c r="J13" s="2">
         <v>44391</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K13" s="2">
+        <v>44392.66666666667</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>44992</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Jessica Bauer</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Eastmsallbuck Creek</t>
+        </is>
+      </c>
+      <c r="F14" s="2">
+        <v>44392</v>
+      </c>
+      <c r="G14" s="2">
+        <v>44392</v>
+      </c>
+      <c r="J14" s="2">
+        <v>44387</v>
+      </c>
+      <c r="K14" s="2">
+        <v>44392.66666666667</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>44997</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Penelope Fields</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Mexe</t>
+        </is>
+      </c>
+      <c r="F15" s="2">
+        <v>44392</v>
+      </c>
+      <c r="G15" s="2">
+        <v>44393</v>
+      </c>
+      <c r="K15" s="2">
         <v>44392.66666666667</v>
       </c>
     </row>

</xml_diff>